<commit_message>
data analytics part 2
</commit_message>
<xml_diff>
--- a/data_analytics/excels/PR.xlsx
+++ b/data_analytics/excels/PR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sweetie/GitHubWorkPlace/VRProject/Framework/data_analytics/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CE42CB-1F38-ED4D-B488-87A32565E49D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6E509C-6FAF-D24D-98D2-07B14593737F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{52FF0F8F-615D-8748-B066-CCEC8DC5818A}"/>
   </bookViews>
@@ -505,9 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A451D9FA-0F24-914F-8228-32961A76B56F}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>